<commit_message>
new data with ependorf tip
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/data-taking-raw/commercial-pipette-data-160224.xlsx
+++ b/data/commerical-Vs-printed-comparison/data-taking-raw/commercial-pipette-data-160224.xlsx
@@ -550,21 +550,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>990.1</v>
+        <v>998.4</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>983.3</v>
+        <v>998.2</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>970.4</v>
+        <v>997.7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -572,21 +572,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>990.4</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>986.6</v>
+        <v>997.2</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1">
         <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>986.9</v>
+        <v>998.2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -594,21 +594,21 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>990.6</v>
+        <v>998.4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>984.6</v>
+        <v>999.6</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1">
         <v>3</v>
       </c>
       <c r="H4" s="1">
-        <v>985.3</v>
+        <v>997.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -616,21 +616,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>984.4</v>
+        <v>1004</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>983.8</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1">
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>983.9</v>
+        <v>996.8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,21 +638,21 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>985.9</v>
+        <v>1004</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>977.5</v>
+        <v>1000.3</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
         <v>5</v>
       </c>
       <c r="H6" s="1">
-        <v>988.7</v>
+        <v>997.7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -702,21 +702,21 @@
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>495.3</v>
+        <v>502.7</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>493.6</v>
+        <v>500</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>491</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -724,21 +724,21 @@
         <v>2</v>
       </c>
       <c r="B11" s="1">
-        <v>494.9</v>
+        <v>502.3</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>495.2</v>
+        <v>501.8</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
         <v>2</v>
       </c>
       <c r="H11" s="1">
-        <v>494.4</v>
+        <v>501.6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -746,21 +746,21 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>496</v>
+        <v>502.1</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
         <v>3</v>
       </c>
       <c r="E12" s="1">
-        <v>496</v>
+        <v>501.4</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1">
         <v>3</v>
       </c>
       <c r="H12" s="1">
-        <v>494.9</v>
+        <v>500.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,21 +768,21 @@
         <v>4</v>
       </c>
       <c r="B13" s="1">
-        <v>496.6</v>
+        <v>502.4</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" s="1">
-        <v>496.2</v>
+        <v>500.5</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
         <v>4</v>
       </c>
       <c r="H13" s="1">
-        <v>497.2</v>
+        <v>501</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -790,21 +790,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>493.9</v>
+        <v>502</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>5</v>
       </c>
       <c r="E14" s="1">
-        <v>494.8</v>
+        <v>502.1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>497.5</v>
+        <v>501.2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -854,21 +854,21 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>202.7</v>
+        <v>203.4</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>202</v>
+        <v>203.7</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>1</v>
       </c>
       <c r="H18" s="1">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -876,21 +876,21 @@
         <v>2</v>
       </c>
       <c r="B19" s="1">
-        <v>202.7</v>
+        <v>203.5</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="1">
-        <v>202.8</v>
+        <v>203.7</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
         <v>2</v>
       </c>
       <c r="H19" s="1">
-        <v>203.9</v>
+        <v>203.8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -898,21 +898,21 @@
         <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>203.5</v>
+        <v>203</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>3</v>
       </c>
       <c r="E20" s="1">
-        <v>202</v>
+        <v>203.8</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1">
         <v>3</v>
       </c>
       <c r="H20" s="1">
-        <v>202.3</v>
+        <v>203.6</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -927,14 +927,14 @@
         <v>4</v>
       </c>
       <c r="E21" s="1">
-        <v>202.5</v>
+        <v>203.5</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
         <v>4</v>
       </c>
       <c r="H21" s="1">
-        <v>200.9</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,21 +942,21 @@
         <v>5</v>
       </c>
       <c r="B22" s="1">
-        <v>202.4</v>
+        <v>203.7</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>5</v>
       </c>
       <c r="E22" s="1">
-        <v>201.1</v>
+        <v>203.8</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
         <v>5</v>
       </c>
       <c r="H22" s="1">
-        <v>203.9</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -994,21 +994,21 @@
         <v>1</v>
       </c>
       <c r="B26" s="1">
-        <v>103</v>
+        <v>104.2</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>103.4</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
         <v>1</v>
       </c>
       <c r="H26" s="1">
-        <v>104.8</v>
+        <v>104.1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,21 +1016,21 @@
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>104.7</v>
+        <v>104.5</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <v>103.6</v>
+        <v>105.6</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
         <v>2</v>
       </c>
       <c r="H27" s="1">
-        <v>103.2</v>
+        <v>104.1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,21 +1038,21 @@
         <v>3</v>
       </c>
       <c r="B28" s="1">
-        <v>104.5</v>
+        <v>104.6</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
         <v>3</v>
       </c>
       <c r="E28" s="1">
-        <v>103.4</v>
+        <v>105.4</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1">
         <v>3</v>
       </c>
       <c r="H28" s="1">
-        <v>103.3</v>
+        <v>104.1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,21 +1060,21 @@
         <v>4</v>
       </c>
       <c r="B29" s="1">
-        <v>103.7</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1">
-        <v>103.3</v>
+        <v>105.1</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1">
         <v>4</v>
       </c>
       <c r="H29" s="1">
-        <v>103.8</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,21 +1082,21 @@
         <v>5</v>
       </c>
       <c r="B30" s="1">
-        <v>103.3</v>
+        <v>104.9</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <v>5</v>
       </c>
       <c r="E30" s="1">
-        <v>103.6</v>
+        <v>104.8</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1">
         <v>5</v>
       </c>
       <c r="H30" s="1">
-        <v>104.5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>